<commit_message>
Render PDF pages as PNG images and extract date from images
</commit_message>
<xml_diff>
--- a/WeeklyMidi.xlsx
+++ b/WeeklyMidi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan.boga\Documents\__Insta-Joliot__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242D99A6-0379-4435-96C7-5099B6161545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092F85F5-9611-4770-AF3D-AA873F18931E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -84,130 +84,112 @@
     <t>Dessert 2</t>
   </si>
   <si>
-    <t>Duo de haricots</t>
-  </si>
-  <si>
     <t>Entree 4</t>
   </si>
   <si>
-    <t>Melon</t>
-  </si>
-  <si>
-    <t>Pastèque</t>
-  </si>
-  <si>
-    <t>Filet de poisson frais</t>
-  </si>
-  <si>
-    <t>16/09</t>
-  </si>
-  <si>
-    <t>17/09</t>
-  </si>
-  <si>
-    <t>18/09</t>
-  </si>
-  <si>
-    <t>19/09</t>
-  </si>
-  <si>
-    <t>20/09</t>
-  </si>
-  <si>
     <t>Pamplemousse</t>
   </si>
   <si>
-    <t>Salade Nantaise</t>
-  </si>
-  <si>
-    <t>Concombre à la crème</t>
-  </si>
-  <si>
-    <t>Saucisse grillée BBC</t>
-  </si>
-  <si>
-    <t>Filet de poisson pané</t>
-  </si>
-  <si>
-    <t>Pommes vapeur</t>
-  </si>
-  <si>
-    <t>Donut</t>
-  </si>
-  <si>
-    <t>Carottes râpées</t>
-  </si>
-  <si>
-    <t>Salade riz au thon</t>
-  </si>
-  <si>
-    <t>Sauté d'agneau au curry</t>
-  </si>
-  <si>
-    <t>Escalope de veau hachée</t>
-  </si>
-  <si>
-    <t>Coquillettes</t>
-  </si>
-  <si>
-    <t>Brocolis</t>
-  </si>
-  <si>
-    <t>Crumble pomme rhubarbe</t>
-  </si>
-  <si>
-    <t>Pizza</t>
+    <t>Couscous bio</t>
+  </si>
+  <si>
+    <t>14/10</t>
+  </si>
+  <si>
+    <t>15/10</t>
+  </si>
+  <si>
+    <t>16/10</t>
+  </si>
+  <si>
+    <t>17/10</t>
+  </si>
+  <si>
+    <t>18/10</t>
+  </si>
+  <si>
+    <t>Tomate mozarella</t>
+  </si>
+  <si>
+    <t>Salade verte parisienne</t>
+  </si>
+  <si>
+    <t>Feuilleté montagnard / VG</t>
+  </si>
+  <si>
+    <t>Pommes bio vapeur</t>
+  </si>
+  <si>
+    <t>Filet de poisson pané MSC</t>
+  </si>
+  <si>
+    <t>Bœuf pot au feu / VG</t>
+  </si>
+  <si>
+    <t>Légumes au pot</t>
+  </si>
+  <si>
+    <t>Tartelette au citron</t>
+  </si>
+  <si>
+    <t>Chicken salade</t>
   </si>
   <si>
     <t>Salade antillaise</t>
   </si>
   <si>
-    <t>Sauté de dinde BBC</t>
-  </si>
-  <si>
-    <t>Gratin de courgette</t>
-  </si>
-  <si>
-    <t>Purée</t>
-  </si>
-  <si>
-    <t>Salade au thon mimosa</t>
-  </si>
-  <si>
-    <t>Terrine de campagne</t>
-  </si>
-  <si>
-    <t>Rôti de porc fumé</t>
-  </si>
-  <si>
-    <t>Galette patate douce lentille</t>
-  </si>
-  <si>
-    <t>Couscous</t>
-  </si>
-  <si>
-    <t>Poêlée de légumes verts</t>
-  </si>
-  <si>
-    <t>Tiramisu maison</t>
-  </si>
-  <si>
-    <t>Tomate sauce tartare</t>
-  </si>
-  <si>
-    <t>Salade de cervelas</t>
-  </si>
-  <si>
-    <t>Bœuf bourguignon</t>
-  </si>
-  <si>
-    <t>Riz pilaf</t>
-  </si>
-  <si>
-    <t>Carottes aux épices</t>
-  </si>
-  <si>
-    <t>Compote de pommes</t>
+    <t>Soupe de légume maison</t>
+  </si>
+  <si>
+    <t>Sauté de lapin à la moutarde</t>
+  </si>
+  <si>
+    <t>Travers de porc braisé</t>
+  </si>
+  <si>
+    <t>Poêlée rustique</t>
+  </si>
+  <si>
+    <t>Salade d'endive aux noix</t>
+  </si>
+  <si>
+    <t>Crumble poireaux jambon / VG</t>
+  </si>
+  <si>
+    <t>Salade athena</t>
+  </si>
+  <si>
+    <t>Lentilles bio</t>
+  </si>
+  <si>
+    <t>Pavé de dinde tandoori</t>
+  </si>
+  <si>
+    <t>Carottes à la crème</t>
+  </si>
+  <si>
+    <t>Panna cotta fruits rouges</t>
+  </si>
+  <si>
+    <t>Betterave bio mimosa</t>
+  </si>
+  <si>
+    <t>Salade exotique</t>
+  </si>
+  <si>
+    <t>Salade drugstore / VG</t>
+  </si>
+  <si>
+    <t>Boulettes de bœuf champignons</t>
+  </si>
+  <si>
+    <t>Spaghettis</t>
+  </si>
+  <si>
+    <t>Boulettes pois chiches bio</t>
+  </si>
+  <si>
+    <t>Épinard béchamel</t>
   </si>
 </sst>
 </file>
@@ -580,7 +562,7 @@
     <col min="8" max="8" width="29" customWidth="1"/>
     <col min="9" max="9" width="26.5703125" customWidth="1"/>
     <col min="10" max="10" width="29.42578125" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -600,7 +582,7 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
@@ -626,34 +608,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -661,34 +619,34 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" t="s">
-        <v>34</v>
-      </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -696,31 +654,31 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
       <c r="I4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -728,34 +686,34 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="I5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="J5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -763,34 +721,31 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="J6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>